<commit_message>
Finally figured out why he appended a character to the string end.
</commit_message>
<xml_diff>
--- a/ExcelEsport/Day4.xlsx
+++ b/ExcelEsport/Day4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{15CA1DAA-FB52-412F-8DFC-598CEAB7A37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E7E657-6B6D-4F23-AD70-1479E2ACB693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>FROM:</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Wildcard Drill</t>
+  </si>
+  <si>
+    <t>The reason to concatenate a character to the string end is to use it as a sentinel for the end. Otherwise, it would match when we con't want it to.</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -541,21 +544,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="14" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -980,7 +982,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1275,7 +1277,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1305,10 +1307,15 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="11">
         <v>45304</v>
       </c>
       <c r="C3" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="23.4" thickBot="1">
       <c r="B8" s="12" t="s">
@@ -1318,24 +1325,24 @@
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="16.8" thickTop="1" thickBot="1">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.2" thickTop="1">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E10" t="b">
@@ -1354,14 +1361,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="31.2">
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:9" ht="15.6">
+      <c r="B11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E11" t="b">
@@ -1381,13 +1388,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.6">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>33</v>
       </c>
       <c r="E12" t="b">
@@ -1407,13 +1414,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.6">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="b">
@@ -1426,13 +1433,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.6">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E14" t="b">
@@ -1445,13 +1452,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.6">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>42</v>
       </c>
       <c r="E15" t="b">
@@ -1464,13 +1471,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.6">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E16" t="b">
@@ -1482,14 +1489,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="46.8">
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="2:6" ht="31.2">
+      <c r="B17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E17" t="b">
@@ -1501,14 +1508,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="31.2">
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="2:6" ht="15.6">
+      <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E18" t="b">
@@ -1521,13 +1528,13 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="31.2">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>54</v>
       </c>
       <c r="E19" t="b">
@@ -1540,13 +1547,13 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.6">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E20" t="b">
@@ -1558,14 +1565,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="31.2">
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="2:6" ht="15.6">
+      <c r="B21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>60</v>
       </c>
       <c r="E21" t="b">
@@ -1624,7 +1631,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Jan-2024</v>
+        <v>20-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1760,19 +1767,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1780,11 +1783,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1792,19 +1794,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1812,11 +1810,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1824,19 +1821,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1844,11 +1837,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1856,13 +1848,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -1935,7 +1927,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>13-Jan-2024</v>
+        <v>20-Jan-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>